<commit_message>
Even more 9 Nov updates
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Library/Mobile Documents/com~apple~CloudDocs/src/empire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACDD41C-124C-6D48-8BDF-E7C21440E842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55311C44-6C11-4F4B-9142-2AC939698198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19960" xr2:uid="{C3BD1D25-DE67-BC4C-A664-0F8B7B384458}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="209">
   <si>
     <t>Command</t>
   </si>
@@ -614,9 +614,6 @@
     <t>Removed</t>
   </si>
   <si>
-    <t>TBD… I think it lists all commands</t>
-  </si>
-  <si>
     <t>A variant of the telegram command. It sends your message to all players</t>
   </si>
   <si>
@@ -632,9 +629,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>N/a</t>
-  </si>
-  <si>
     <t>find out the communications status of a country</t>
   </si>
   <si>
@@ -648,6 +642,27 @@
   </si>
   <si>
     <t>get a list of subjects containing the word you are looking for,</t>
+  </si>
+  <si>
+    <t>List all available commands</t>
+  </si>
+  <si>
+    <t>Add new Nations…. Not something we'll be doing in V</t>
+  </si>
+  <si>
+    <t>load nukes on planes or missiles</t>
+  </si>
+  <si>
+    <t>Loading/Unloading</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Success/fail</t>
+  </si>
+  <si>
+    <t>Specify groupings of land units</t>
   </si>
 </sst>
 </file>
@@ -1037,14 +1052,15 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1053,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>190</v>
@@ -1068,7 +1084,7 @@
         <v>189</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1076,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
         <v>184</v>
@@ -1091,7 +1107,7 @@
         <v>188</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1099,10 +1115,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
         <v>191</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1110,10 +1129,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
+        <v>188</v>
       </c>
       <c r="F4" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="G4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1121,7 +1152,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
         <v>184</v>
@@ -1136,7 +1167,7 @@
         <v>188</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1144,10 +1175,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
         <v>188</v>
@@ -1159,7 +1190,7 @@
         <v>188</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1167,10 +1198,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
         <v>186</v>
@@ -1182,17 +1213,53 @@
         <v>188</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates from the day of 10 Nov
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Library/Mobile Documents/com~apple~CloudDocs/src/empire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55311C44-6C11-4F4B-9142-2AC939698198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C36485-1F21-F844-80BE-2755BF9F6FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19960" xr2:uid="{C3BD1D25-DE67-BC4C-A664-0F8B7B384458}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="212">
   <si>
     <t>Command</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>Specify groupings of land units</t>
+  </si>
+  <si>
+    <t>Combat</t>
+  </si>
+  <si>
+    <t>From MaritimeUnit to LandUnits</t>
+  </si>
+  <si>
+    <t>BTUs</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E50B8-623E-EC4D-86F5-D27104B84908}">
-  <dimension ref="A1:G184"/>
+  <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,11 +1069,11 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,10 +1093,13 @@
         <v>189</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1106,11 +1118,11 @@
       <c r="F2" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1120,11 +1132,11 @@
       <c r="F3" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1143,11 +1155,11 @@
       <c r="F4" t="s">
         <v>188</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1166,11 +1178,11 @@
       <c r="F5" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1189,11 +1201,11 @@
       <c r="F6" t="s">
         <v>188</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1212,11 +1224,11 @@
       <c r="F7" t="s">
         <v>188</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1235,11 +1247,11 @@
       <c r="F8" t="s">
         <v>188</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1258,41 +1270,59 @@
       <c r="F9" t="s">
         <v>188</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Updates for 11 Nov
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Library/Mobile Documents/com~apple~CloudDocs/src/empire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C36485-1F21-F844-80BE-2755BF9F6FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD7728-30A7-BB41-83C8-FD1C7E0ACA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19960" xr2:uid="{C3BD1D25-DE67-BC4C-A664-0F8B7B384458}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="250">
   <si>
     <t>Command</t>
   </si>
@@ -647,9 +647,6 @@
     <t>List all available commands</t>
   </si>
   <si>
-    <t>Add new Nations…. Not something we'll be doing in V</t>
-  </si>
-  <si>
     <t>load nukes on planes or missiles</t>
   </si>
   <si>
@@ -672,6 +669,123 @@
   </si>
   <si>
     <t>BTUs</t>
+  </si>
+  <si>
+    <t>From Land to Land</t>
+  </si>
+  <si>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>shows you the best path from any sector to any sector</t>
+  </si>
+  <si>
+    <t>Override a sector in your NationalView (say, to mark a minefield)</t>
+  </si>
+  <si>
+    <t>reflects everything you've learned about the world</t>
+  </si>
+  <si>
+    <t>Attack from one ship to another</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Attack from air to ship, land units and sectors</t>
+  </si>
+  <si>
+    <t>removes the sanctuary protection from your country and forces your people to work for a living</t>
+  </si>
+  <si>
+    <t>Nation</t>
+  </si>
+  <si>
+    <t>predicts expenses and income for the next update</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>ClassFactory</t>
+  </si>
+  <si>
+    <t>Mostly</t>
+  </si>
+  <si>
+    <t>build ships, planes, land units and nukes in your harbors, airfields, headquarters and nuclear plants</t>
+  </si>
+  <si>
+    <t>purchase commodities on the open market</t>
+  </si>
+  <si>
+    <t>Commerce</t>
+  </si>
+  <si>
+    <t>End a session</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Sectors</t>
+  </si>
+  <si>
+    <t>Change the location of your capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lists the commodities on board your ships </t>
+  </si>
+  <si>
+    <t>display specific information on some of the sectors you occupy</t>
+  </si>
+  <si>
+    <t>rename your country, or your representative</t>
+  </si>
+  <si>
+    <t>allows coastal sectors to report sightings of ships</t>
+  </si>
+  <si>
+    <t>Loans</t>
+  </si>
+  <si>
+    <t>seize one or more of his/her sectors</t>
+  </si>
+  <si>
+    <t>provides information pertaining to the various commodities in the sectors you occupy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> consider accepting a loan offered by another country.</t>
+  </si>
+  <si>
+    <t>converts enemy (captured) populace into uncompensated workers</t>
+  </si>
+  <si>
+    <t>Commodities</t>
+  </si>
+  <si>
+    <t>displays status of countries</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>provides information about the various delivery cutoff levels</t>
+  </si>
+  <si>
+    <t>officially declare your diplomatic relations with other countries</t>
+  </si>
+  <si>
+    <t>fine tune a distribution network</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Add new Nations…. Something we'll won't do in V</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E50B8-623E-EC4D-86F5-D27104B84908}">
   <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1207,7 @@
         <v>189</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>193</v>
@@ -1129,11 +1243,20 @@
       <c r="B3" t="s">
         <v>194</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="F3" t="s">
         <v>191</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1236,19 +1359,19 @@
         <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" t="s">
         <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" t="s">
         <v>188</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1259,19 +1382,19 @@
         <v>194</v>
       </c>
       <c r="C9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
         <v>206</v>
       </c>
-      <c r="D9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="F9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1282,207 +1405,642 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H10" t="s">
         <v>209</v>
-      </c>
-      <c r="D10" t="s">
-        <v>188</v>
-      </c>
-      <c r="E10" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H10" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+      <c r="H11" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" t="s">
+        <v>188</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" t="s">
+        <v>188</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" t="s">
+        <v>188</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" t="s">
+        <v>186</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" t="s">
+        <v>225</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
+        <v>228</v>
+      </c>
+      <c r="D20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" t="s">
+        <v>188</v>
+      </c>
+      <c r="H22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" t="s">
+        <v>188</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" t="s">
+        <v>188</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" t="s">
+        <v>188</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" t="s">
+        <v>188</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" t="s">
+        <v>188</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" t="s">
+        <v>242</v>
+      </c>
+      <c r="D30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" t="s">
+        <v>244</v>
+      </c>
+      <c r="D32" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" t="s">
+        <v>188</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" t="s">
+        <v>188</v>
+      </c>
+      <c r="E33" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" t="s">
+        <v>188</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>

</xml_diff>